<commit_message>
LATEST SUPPOSEDLY STABLE VERSION
</commit_message>
<xml_diff>
--- a/Files/0000-1000/6/A6_RequestList.xlsx
+++ b/Files/0000-1000/6/A6_RequestList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">ФК 404-4   </t>
   </si>
@@ -58,15 +58,15 @@
     <t>Млечно изследване 2</t>
   </si>
   <si>
+    <t>БДС 0001 АР</t>
+  </si>
+  <si>
+    <t>489</t>
+  </si>
+  <si>
     <t>БНС 1234 АМ</t>
   </si>
   <si>
-    <t>489</t>
-  </si>
-  <si>
-    <t>БДС 0001 АР</t>
-  </si>
-  <si>
     <t>2. Кокоши яйца</t>
   </si>
   <si>
@@ -76,9 +76,6 @@
     <t>БДС 11425</t>
   </si>
   <si>
-    <t>БДС ХЕР7</t>
-  </si>
-  <si>
     <t>3. Печен фъстък</t>
   </si>
   <si>
@@ -91,16 +88,22 @@
     <t>4. Свинско месо</t>
   </si>
   <si>
+    <t>Киселинност</t>
+  </si>
+  <si>
+    <t>БДС 456АЕЕР</t>
+  </si>
+  <si>
+    <t>БДС 7894</t>
+  </si>
+  <si>
+    <t>Забележка ...</t>
+  </si>
+  <si>
     <t>Ешерихия коли</t>
   </si>
   <si>
-    <t>БДС 753691</t>
-  </si>
-  <si>
-    <t>Киселинност</t>
-  </si>
-  <si>
-    <t>БДС 456АЕЕР</t>
+    <t>БДС 788А</t>
   </si>
   <si>
     <t>Срок за изпитване: 5 дни</t>
@@ -671,12 +674,14 @@
     </row>
     <row r="13">
       <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="11"/>
@@ -684,61 +689,61 @@
     <row r="14">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="11"/>
     </row>
     <row r="15">
       <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11"/>
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>